<commit_message>
cap nhat file phan chia cong viec
</commit_message>
<xml_diff>
--- a/Phanchiacongviec.xlsx
+++ b/Phanchiacongviec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daochinam/Cybersoft/FrontEnd/Project/bc55_BS4_NamDao_SangDang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79337324-D9E1-B746-8B1D-FC6794C011EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A086066-8A93-8945-B7EA-80C4B0E182AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37120" yWindow="2960" windowWidth="28040" windowHeight="16940" xr2:uid="{8976448D-8208-3C4D-B324-87CA2C40994C}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,7 +567,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -603,7 +603,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -639,7 +639,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -652,12 +652,12 @@
         <v>14</v>
       </c>
       <c r="B8" s="4">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="4">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="2"/>
@@ -688,12 +688,12 @@
         <v>16</v>
       </c>
       <c r="B10" s="4">
-        <v>45156</v>
+        <v>45154</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -706,7 +706,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="4">
-        <v>45156</v>
+        <v>45154</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
@@ -724,12 +724,12 @@
         <v>18</v>
       </c>
       <c r="B12" s="4">
-        <v>45157</v>
+        <v>45154</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -742,7 +742,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="4">
-        <v>45157</v>
+        <v>45154</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2"/>

</xml_diff>

<commit_message>
update pj lan cuoi
</commit_message>
<xml_diff>
--- a/Phanchiacongviec.xlsx
+++ b/Phanchiacongviec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daochinam/Cybersoft/FrontEnd/Project/bc55_BS4_NamDao_SangDang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A086066-8A93-8945-B7EA-80C4B0E182AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9A70F0-A93A-0447-A73C-3E073609FE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37120" yWindow="2960" windowWidth="28040" windowHeight="16940" xr2:uid="{8976448D-8208-3C4D-B324-87CA2C40994C}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Task Name</t>
   </si>
@@ -95,9 +94,6 @@
     <t xml:space="preserve">    11 footer </t>
   </si>
   <si>
-    <t xml:space="preserve">    12 theme + right header </t>
-  </si>
-  <si>
     <t xml:space="preserve">      2 Hero Header </t>
   </si>
   <si>
@@ -105,6 +101,12 @@
   </si>
   <si>
     <t>sangdang</t>
+  </si>
+  <si>
+    <t>    12 theme + right header + backtotop</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -126,7 +128,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +138,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -175,6 +183,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,12 +506,12 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
@@ -546,10 +560,12 @@
       <c r="B2" s="4">
         <v>45152</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -559,15 +575,17 @@
     </row>
     <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4">
         <v>45152</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -582,10 +600,12 @@
       <c r="B4" s="4">
         <v>45153</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -600,10 +620,12 @@
       <c r="B5" s="4">
         <v>45153</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -618,10 +640,12 @@
       <c r="B6" s="4">
         <v>45154</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -636,10 +660,12 @@
       <c r="B7" s="4">
         <v>45154</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -648,112 +674,184 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>45154</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="C8" s="6">
+        <v>45158</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="6">
+        <v>45157</v>
+      </c>
+      <c r="G8" s="6">
+        <v>45158</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="6">
         <v>45154</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="C9" s="6">
+        <v>45158</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="6">
+        <v>45157</v>
+      </c>
+      <c r="G9" s="6">
+        <v>45158</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="6">
         <v>45154</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="C10" s="6">
+        <v>45158</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="6">
+        <v>45157</v>
+      </c>
+      <c r="G10" s="6">
+        <v>45158</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="6">
         <v>45154</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="C11" s="6">
+        <v>45158</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="6">
+        <v>45157</v>
+      </c>
+      <c r="G11" s="6">
+        <v>45158</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="6">
         <v>45154</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="C12" s="6">
+        <v>45158</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="6">
+        <v>45157</v>
+      </c>
+      <c r="G12" s="6">
+        <v>45158</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6">
         <v>45154</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="C13" s="6">
+        <v>45158</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="6">
+        <v>45157</v>
+      </c>
+      <c r="G13" s="6">
+        <v>45158</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>